<commit_message>
Fix  Mem Small + fileOutput
</commit_message>
<xml_diff>
--- a/Diagrama.xlsx
+++ b/Diagrama.xlsx
@@ -909,6 +909,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -925,12 +991,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="2" applyBorder="1" applyAlignment="1">
@@ -972,18 +1032,6 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -999,12 +1047,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1019,48 +1061,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="34" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1353,7 +1353,7 @@
   <dimension ref="A1:S67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1378,13 +1378,13 @@
       <c r="A1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="84" t="s">
+      <c r="B1" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="85"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="53"/>
       <c r="G1" s="29" t="s">
         <v>22</v>
       </c>
@@ -1399,13 +1399,13 @@
       <c r="A2" s="17">
         <v>1</v>
       </c>
-      <c r="B2" s="86" t="s">
+      <c r="B2" s="54" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="88"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="31">
         <v>150</v>
       </c>
@@ -1420,13 +1420,13 @@
       <c r="A3" s="17">
         <v>2</v>
       </c>
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="77"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="47"/>
       <c r="G3" s="32">
         <v>150</v>
       </c>
@@ -1441,13 +1441,13 @@
       <c r="A4" s="17">
         <v>3</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="92"/>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="93"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="64"/>
       <c r="G4" s="32">
         <v>150</v>
       </c>
@@ -1485,13 +1485,13 @@
       <c r="A5" s="17">
         <v>4</v>
       </c>
-      <c r="B5" s="94" t="s">
+      <c r="B5" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="70"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
       <c r="G5" s="32">
         <v>150</v>
       </c>
@@ -1529,15 +1529,15 @@
       <c r="A6" s="17">
         <v>5</v>
       </c>
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="53"/>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="32">
         <v>122</v>
       </c>
@@ -1563,13 +1563,13 @@
       <c r="A7" s="17">
         <v>6</v>
       </c>
-      <c r="B7" s="96"/>
-      <c r="C7" s="68" t="s">
+      <c r="B7" s="67"/>
+      <c r="C7" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="70"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="51"/>
       <c r="G7" s="32">
         <v>122</v>
       </c>
@@ -1594,15 +1594,15 @@
       <c r="A8" s="17">
         <v>7</v>
       </c>
-      <c r="B8" s="96"/>
-      <c r="C8" s="56" t="s">
+      <c r="B8" s="67"/>
+      <c r="C8" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="76" t="s">
+      <c r="D8" s="77"/>
+      <c r="E8" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="77"/>
+      <c r="F8" s="47"/>
       <c r="G8" s="32">
         <v>48</v>
       </c>
@@ -1627,13 +1627,13 @@
       <c r="A9" s="17">
         <v>8</v>
       </c>
-      <c r="B9" s="96"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="52" t="s">
+      <c r="B9" s="67"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="53"/>
+      <c r="F9" s="61"/>
       <c r="G9" s="32">
         <v>48</v>
       </c>
@@ -1658,13 +1658,13 @@
       <c r="A10" s="17">
         <v>9</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="76" t="s">
+      <c r="B10" s="67"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="77"/>
+      <c r="F10" s="47"/>
       <c r="G10" s="32">
         <v>48</v>
       </c>
@@ -1677,13 +1677,13 @@
       <c r="A11" s="17">
         <v>10</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="76" t="s">
+      <c r="B11" s="67"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="79"/>
+      <c r="E11" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="77"/>
+      <c r="F11" s="47"/>
       <c r="G11" s="32">
         <v>48</v>
       </c>
@@ -1696,13 +1696,13 @@
       <c r="A12" s="17">
         <v>11</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="78" t="s">
+      <c r="B12" s="67"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="79"/>
+      <c r="F12" s="93"/>
       <c r="G12" s="32">
         <v>48</v>
       </c>
@@ -1715,13 +1715,13 @@
       <c r="A13" s="17">
         <v>12</v>
       </c>
-      <c r="B13" s="96"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="59"/>
-      <c r="E13" s="76" t="s">
+      <c r="B13" s="67"/>
+      <c r="C13" s="78"/>
+      <c r="D13" s="79"/>
+      <c r="E13" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="77"/>
+      <c r="F13" s="47"/>
       <c r="G13" s="32">
         <v>48</v>
       </c>
@@ -1729,13 +1729,13 @@
       <c r="I13" s="24">
         <v>3</v>
       </c>
-      <c r="K13" s="83" t="s">
+      <c r="K13" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="L13" s="83"/>
+      <c r="L13" s="48"/>
       <c r="M13" s="26">
-        <f>SUM(G2:G23)</f>
-        <v>1922</v>
+        <f>SUM(G2:G22)</f>
+        <v>1900</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1743,12 +1743,12 @@
         <v>13</v>
       </c>
       <c r="B14" s="33"/>
-      <c r="C14" s="58"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="76" t="s">
+      <c r="C14" s="78"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="77"/>
+      <c r="F14" s="47"/>
       <c r="G14" s="32">
         <v>48</v>
       </c>
@@ -1769,12 +1769,12 @@
       <c r="B15" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="58"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="76" t="s">
+      <c r="C15" s="78"/>
+      <c r="D15" s="79"/>
+      <c r="E15" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="77"/>
+      <c r="F15" s="47"/>
       <c r="G15" s="32">
         <v>76</v>
       </c>
@@ -1790,12 +1790,12 @@
       <c r="B16" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="60"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="74" t="s">
+      <c r="C16" s="80"/>
+      <c r="D16" s="81"/>
+      <c r="E16" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="75"/>
+      <c r="F16" s="91"/>
       <c r="G16" s="32">
         <v>76</v>
       </c>
@@ -1806,17 +1806,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="17">
         <v>16</v>
       </c>
-      <c r="B17" s="71" t="s">
+      <c r="B17" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="67"/>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="53"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="61"/>
       <c r="G17" s="32">
         <v>150</v>
       </c>
@@ -1825,17 +1825,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17">
         <v>17</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C18" s="73"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="70"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="51"/>
       <c r="G18" s="32">
         <v>150</v>
       </c>
@@ -1843,19 +1843,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="17">
         <v>18</v>
       </c>
-      <c r="B19" s="62" t="s">
+      <c r="B19" s="82" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="63"/>
-      <c r="D19" s="52" t="s">
+      <c r="C19" s="83"/>
+      <c r="D19" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="67"/>
-      <c r="F19" s="53"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="61"/>
       <c r="G19" s="32">
         <v>77</v>
       </c>
@@ -1864,17 +1864,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17">
         <v>19</v>
       </c>
-      <c r="B20" s="64"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="68" t="s">
+      <c r="B20" s="84"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="69"/>
-      <c r="F20" s="70"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="51"/>
       <c r="G20" s="32">
         <v>77</v>
       </c>
@@ -1883,19 +1883,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="17">
         <v>20</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="46" t="s">
+      <c r="B21" s="84"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="52" t="s">
+      <c r="E21" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="53"/>
+      <c r="F21" s="61"/>
       <c r="G21" s="32">
         <v>57</v>
       </c>
@@ -1904,17 +1904,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17">
         <v>21</v>
       </c>
-      <c r="B22" s="64"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="47"/>
-      <c r="E22" s="68" t="s">
+      <c r="B22" s="84"/>
+      <c r="C22" s="86"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="F22" s="70"/>
+      <c r="F22" s="51"/>
       <c r="G22" s="32">
         <v>57</v>
       </c>
@@ -1922,15 +1922,16 @@
       <c r="I22" s="24">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="N22" s="21"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="17">
         <v>22</v>
       </c>
-      <c r="B23" s="64"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="48"/>
-      <c r="E23" s="80" t="s">
+      <c r="B23" s="84"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="70"/>
+      <c r="E23" s="94" t="s">
         <v>15</v>
       </c>
       <c r="F23" s="38" t="s">
@@ -1943,14 +1944,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="17">
         <v>23</v>
       </c>
-      <c r="B24" s="64"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="48"/>
-      <c r="E24" s="81"/>
+      <c r="B24" s="84"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="95"/>
       <c r="F24" s="39" t="s">
         <v>24</v>
       </c>
@@ -1962,14 +1963,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="17">
         <v>24</v>
       </c>
-      <c r="B25" s="64"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="48"/>
-      <c r="E25" s="81"/>
+      <c r="B25" s="84"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="95"/>
       <c r="F25" s="39" t="s">
         <v>24</v>
       </c>
@@ -1981,14 +1982,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="17">
         <v>25</v>
       </c>
-      <c r="B26" s="64"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="48"/>
-      <c r="E26" s="81"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="95"/>
       <c r="F26" s="39" t="s">
         <v>24</v>
       </c>
@@ -2000,14 +2001,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="17">
         <v>26</v>
       </c>
-      <c r="B27" s="64"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="48"/>
-      <c r="E27" s="81"/>
+      <c r="B27" s="84"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="95"/>
       <c r="F27" s="39" t="s">
         <v>24</v>
       </c>
@@ -2019,14 +2020,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="17">
         <v>27</v>
       </c>
-      <c r="B28" s="64"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="48"/>
-      <c r="E28" s="81"/>
+      <c r="B28" s="84"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="70"/>
+      <c r="E28" s="95"/>
       <c r="F28" s="39" t="s">
         <v>24</v>
       </c>
@@ -2038,14 +2039,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="17">
         <v>28</v>
       </c>
-      <c r="B29" s="64"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="48"/>
-      <c r="E29" s="81"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="70"/>
+      <c r="E29" s="95"/>
       <c r="F29" s="39" t="s">
         <v>24</v>
       </c>
@@ -2057,14 +2058,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="17">
         <v>29</v>
       </c>
-      <c r="B30" s="64"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="48"/>
-      <c r="E30" s="81"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="70"/>
+      <c r="E30" s="95"/>
       <c r="F30" s="39" t="s">
         <v>24</v>
       </c>
@@ -2076,14 +2077,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="17">
         <v>30</v>
       </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="66"/>
+      <c r="B31" s="84"/>
+      <c r="C31" s="86"/>
       <c r="D31" s="40"/>
-      <c r="E31" s="81"/>
+      <c r="E31" s="95"/>
       <c r="F31" s="39" t="s">
         <v>24</v>
       </c>
@@ -2097,16 +2098,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="17">
         <v>31</v>
       </c>
-      <c r="B32" s="64"/>
-      <c r="C32" s="66"/>
+      <c r="B32" s="84"/>
+      <c r="C32" s="86"/>
       <c r="D32" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="81"/>
+      <c r="E32" s="95"/>
       <c r="F32" s="39" t="s">
         <v>24</v>
       </c>
@@ -2122,12 +2123,12 @@
       <c r="A33" s="17">
         <v>32</v>
       </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="66"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="86"/>
       <c r="D33" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="81"/>
+      <c r="E33" s="95"/>
       <c r="F33" s="39" t="s">
         <v>24</v>
       </c>
@@ -2143,12 +2144,12 @@
       <c r="A34" s="17">
         <v>33</v>
       </c>
-      <c r="B34" s="54"/>
-      <c r="C34" s="55"/>
+      <c r="B34" s="74"/>
+      <c r="C34" s="75"/>
       <c r="D34" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="82"/>
+      <c r="E34" s="96"/>
       <c r="F34" s="39" t="s">
         <v>24</v>
       </c>
@@ -2166,11 +2167,11 @@
       <c r="A35" s="17">
         <v>34</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="50"/>
-      <c r="D35" s="51"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="73"/>
       <c r="E35" s="41"/>
       <c r="F35" s="42" t="s">
         <v>24</v>
@@ -2395,6 +2396,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="C8:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B19:C33"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E23:E34"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="C7:F7"/>
@@ -2411,21 +2427,6 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:B13"/>
     <mergeCell ref="D21:D30"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="C8:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B19:C33"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E23:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>